<commit_message>
add collection_method to pH water sampling
</commit_message>
<xml_diff>
--- a/pH_glider/water_sampling/sample_logs/RMI2_pH_Water_Sample_Log.xlsx
+++ b/pH_glider/water_sampling/sample_logs/RMI2_pH_Water_Sample_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garzio/Documents/repo/rucool/dataset_archiving/pH_glider/water_sampling/sample_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F02C5FC-0BEF-CD42-8A35-F11E094F4E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376FDD8C-559F-4C4F-B334-3E0391135217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37260" yWindow="500" windowWidth="35840" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17080" yWindow="500" windowWidth="20800" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleLog" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
   <si>
-    <t>Deployment Notes</t>
-  </si>
-  <si>
     <t>Sample #</t>
   </si>
   <si>
@@ -169,7 +166,10 @@
     <t>single niskin</t>
   </si>
   <si>
-    <t>Had issues with rosette, captured the rest of the samples with a single niskin. Temp/salinity are from the glider</t>
+    <t>Collection method</t>
+  </si>
+  <si>
+    <t>single_niskin</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13:R13"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -544,113 +544,113 @@
     <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.1640625" customWidth="1"/>
-    <col min="26" max="26" width="59" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
       </c>
       <c r="E2" s="3">
         <v>45770</v>
@@ -671,7 +671,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -679,37 +679,37 @@
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="N2">
+      <c r="N2" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2">
         <v>500</v>
       </c>
-      <c r="O2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2">
+      <c r="P2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2">
         <v>14</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>6.8342000000000001</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>30.8078</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
       </c>
       <c r="E3" s="3">
         <v>45770</v>
@@ -730,7 +730,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -738,37 +738,37 @@
       <c r="M3">
         <v>1</v>
       </c>
-      <c r="N3">
+      <c r="N3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3">
         <v>500</v>
       </c>
-      <c r="O3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3">
+      <c r="P3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3">
         <v>14</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>6.8342000000000001</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>30.8078</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
       </c>
       <c r="E4" s="3">
         <v>45770</v>
@@ -789,7 +789,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -797,37 +797,37 @@
       <c r="M4">
         <v>3</v>
       </c>
-      <c r="N4">
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4">
         <v>500</v>
       </c>
-      <c r="O4" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4">
+      <c r="P4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4">
         <v>7</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>8.2327999999999992</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>28.705300000000001</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
       </c>
       <c r="E5" s="3">
         <v>45770</v>
@@ -848,7 +848,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -856,37 +856,37 @@
       <c r="M5">
         <v>3</v>
       </c>
-      <c r="N5">
+      <c r="N5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5">
         <v>500</v>
       </c>
-      <c r="O5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P5">
+      <c r="P5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5">
         <v>7</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>8.2327999999999992</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>28.705300000000001</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
       </c>
       <c r="E6" s="3">
         <v>45770</v>
@@ -907,7 +907,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L6">
         <v>2</v>
@@ -915,37 +915,37 @@
       <c r="M6">
         <v>1</v>
       </c>
-      <c r="N6">
+      <c r="N6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O6">
         <v>500</v>
       </c>
-      <c r="O6" t="s">
-        <v>43</v>
-      </c>
-      <c r="P6">
+      <c r="P6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6">
         <v>2</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>9.7957999999999998</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>26.1554</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
       </c>
       <c r="E7" s="3">
         <v>45770</v>
@@ -966,7 +966,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7">
         <v>2</v>
@@ -974,37 +974,37 @@
       <c r="M7">
         <v>1</v>
       </c>
-      <c r="N7">
+      <c r="N7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7">
         <v>500</v>
       </c>
-      <c r="O7" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7">
+      <c r="P7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7">
         <v>2</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>9.7957999999999998</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>26.1554</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
       </c>
       <c r="E8" s="3">
         <v>45770</v>
@@ -1025,7 +1025,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -1033,37 +1033,37 @@
       <c r="M8">
         <v>1</v>
       </c>
-      <c r="N8">
+      <c r="N8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8">
         <v>500</v>
       </c>
-      <c r="O8" t="s">
-        <v>43</v>
-      </c>
-      <c r="P8">
+      <c r="P8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8">
         <v>7</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>8.2327999999999992</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>28.705300000000001</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
       </c>
       <c r="E9" s="3">
         <v>45770</v>
@@ -1084,7 +1084,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L9">
         <v>3</v>
@@ -1092,37 +1092,37 @@
       <c r="M9">
         <v>1</v>
       </c>
-      <c r="N9">
+      <c r="N9" t="s">
+        <v>44</v>
+      </c>
+      <c r="O9">
         <v>500</v>
       </c>
-      <c r="O9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P9">
+      <c r="P9" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9">
         <v>7</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>8.2327999999999992</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>28.705300000000001</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
       </c>
       <c r="E10" s="3">
         <v>45770</v>
@@ -1143,7 +1143,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L10">
         <v>4</v>
@@ -1151,37 +1151,37 @@
       <c r="M10">
         <v>1</v>
       </c>
-      <c r="N10">
+      <c r="N10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10">
         <v>500</v>
       </c>
-      <c r="O10" t="s">
-        <v>43</v>
-      </c>
-      <c r="P10">
+      <c r="P10" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10">
         <v>14</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>6.8342000000000001</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>30.8078</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
       </c>
       <c r="E11" s="3">
         <v>45770</v>
@@ -1202,7 +1202,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L11">
         <v>4</v>
@@ -1210,37 +1210,37 @@
       <c r="M11">
         <v>1</v>
       </c>
-      <c r="N11">
+      <c r="N11" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11">
         <v>500</v>
       </c>
-      <c r="O11" t="s">
-        <v>43</v>
-      </c>
-      <c r="P11">
+      <c r="P11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q11">
         <v>14</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>6.8342000000000001</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>30.8078</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
       </c>
       <c r="E12" s="3">
         <v>45770</v>
@@ -1261,7 +1261,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L12">
         <v>5</v>
@@ -1269,37 +1269,37 @@
       <c r="M12">
         <v>1</v>
       </c>
-      <c r="N12">
+      <c r="N12" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12">
         <v>500</v>
       </c>
-      <c r="O12" t="s">
-        <v>43</v>
-      </c>
-      <c r="P12">
+      <c r="P12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12">
         <v>2</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>9.7957999999999998</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>26.1554</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
       </c>
       <c r="E13" s="3">
         <v>45770</v>
@@ -1320,7 +1320,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L13">
         <v>5</v>
@@ -1328,23 +1328,23 @@
       <c r="M13">
         <v>1</v>
       </c>
-      <c r="N13">
+      <c r="N13" t="s">
+        <v>44</v>
+      </c>
+      <c r="O13">
         <v>500</v>
       </c>
-      <c r="O13" t="s">
-        <v>43</v>
-      </c>
-      <c r="P13">
+      <c r="P13" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13">
         <v>2</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>9.7957999999999998</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>26.1554</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add pH QC to dataset
</commit_message>
<xml_diff>
--- a/pH_glider/water_sampling/sample_logs/RMI2_pH_Water_Sample_Log.xlsx
+++ b/pH_glider/water_sampling/sample_logs/RMI2_pH_Water_Sample_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garzio/Documents/repo/rucool/dataset_archiving/pH_glider/water_sampling/sample_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762A67D1-2696-5140-A675-38E1C7621607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE2268B-AA45-7647-B340-AD594A4F478C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="500" windowWidth="34520" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34520" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleLog" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="76">
   <si>
     <t>Sample #</t>
   </si>
@@ -61,18 +61,6 @@
     <t>pH Stdev</t>
   </si>
   <si>
-    <t>Average TA</t>
-  </si>
-  <si>
-    <t>TA Stdev</t>
-  </si>
-  <si>
-    <t>Average DIC</t>
-  </si>
-  <si>
-    <t>DIC Stdev</t>
-  </si>
-  <si>
     <t>Station ID</t>
   </si>
   <si>
@@ -254,6 +242,27 @@
   </si>
   <si>
     <t>rosette bottles didn't close, so collected this sample immediately after rosette on board with single_niskin; ctd data from ctd profile not bottle file. CTD was on rosette</t>
+  </si>
+  <si>
+    <t>Average DIC (umol/kg)</t>
+  </si>
+  <si>
+    <t>DIC Stdev (umol/kg)</t>
+  </si>
+  <si>
+    <t>Average TA (umol/kg)</t>
+  </si>
+  <si>
+    <t>TA Stdev (umol/kg)</t>
+  </si>
+  <si>
+    <t>pH_from_DIC_TA_total_25C</t>
+  </si>
+  <si>
+    <t>pH(measured-calculated)</t>
+  </si>
+  <si>
+    <t>pH_flag</t>
   </si>
 </sst>
 </file>
@@ -606,11 +615,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z37"/>
+  <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M29" sqref="M29"/>
+      <selection pane="bottomLeft" activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -636,43 +645,46 @@
     <col min="19" max="19" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.1640625" customWidth="1"/>
+    <col min="22" max="22" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>0</v>
@@ -681,13 +693,13 @@
         <v>1</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>4</v>
@@ -708,33 +720,42 @@
         <v>7</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3">
         <v>45770</v>
@@ -755,7 +776,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -764,13 +785,13 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O2">
         <v>500</v>
       </c>
       <c r="P2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Q2">
         <v>14</v>
@@ -782,18 +803,18 @@
         <v>30.8078</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3">
         <v>45770</v>
@@ -814,7 +835,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -823,13 +844,13 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O3">
         <v>500</v>
       </c>
       <c r="P3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Q3">
         <v>14</v>
@@ -841,18 +862,18 @@
         <v>30.8078</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3">
         <v>45770</v>
@@ -873,7 +894,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -882,13 +903,13 @@
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O4">
         <v>500</v>
       </c>
       <c r="P4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Q4">
         <v>7</v>
@@ -900,18 +921,18 @@
         <v>28.705300000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3">
         <v>45770</v>
@@ -932,7 +953,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -941,13 +962,13 @@
         <v>3</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O5">
         <v>500</v>
       </c>
       <c r="P5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Q5">
         <v>7</v>
@@ -959,18 +980,18 @@
         <v>28.705300000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E6" s="3">
         <v>45770</v>
@@ -991,7 +1012,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L6">
         <v>2</v>
@@ -1000,13 +1021,13 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O6">
         <v>500</v>
       </c>
       <c r="P6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q6">
         <v>2</v>
@@ -1018,18 +1039,18 @@
         <v>26.1554</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3">
         <v>45770</v>
@@ -1050,7 +1071,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L7">
         <v>2</v>
@@ -1059,13 +1080,13 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O7">
         <v>500</v>
       </c>
       <c r="P7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q7">
         <v>2</v>
@@ -1077,18 +1098,18 @@
         <v>26.1554</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3">
         <v>45770</v>
@@ -1109,7 +1130,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -1118,13 +1139,13 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O8">
         <v>500</v>
       </c>
       <c r="P8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q8">
         <v>7</v>
@@ -1136,18 +1157,18 @@
         <v>28.705300000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E9" s="3">
         <v>45770</v>
@@ -1168,7 +1189,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L9">
         <v>3</v>
@@ -1177,13 +1198,13 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O9">
         <v>500</v>
       </c>
       <c r="P9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q9">
         <v>7</v>
@@ -1195,18 +1216,18 @@
         <v>28.705300000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E10" s="3">
         <v>45770</v>
@@ -1227,7 +1248,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L10">
         <v>4</v>
@@ -1236,13 +1257,13 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O10">
         <v>500</v>
       </c>
       <c r="P10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q10">
         <v>14</v>
@@ -1254,18 +1275,18 @@
         <v>30.8078</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E11" s="3">
         <v>45770</v>
@@ -1286,7 +1307,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L11">
         <v>4</v>
@@ -1295,13 +1316,13 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O11">
         <v>500</v>
       </c>
       <c r="P11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q11">
         <v>14</v>
@@ -1313,18 +1334,18 @@
         <v>30.8078</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E12" s="3">
         <v>45770</v>
@@ -1345,7 +1366,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L12">
         <v>5</v>
@@ -1354,13 +1375,13 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O12">
         <v>500</v>
       </c>
       <c r="P12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q12">
         <v>2</v>
@@ -1372,18 +1393,18 @@
         <v>26.1554</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E13" s="3">
         <v>45770</v>
@@ -1404,7 +1425,7 @@
         <v>51.177999999999997</v>
       </c>
       <c r="K13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="L13">
         <v>5</v>
@@ -1413,13 +1434,13 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O13">
         <v>500</v>
       </c>
       <c r="P13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q13">
         <v>2</v>
@@ -1431,18 +1452,18 @@
         <v>26.1554</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E14" s="3">
         <v>45797</v>
@@ -1463,7 +1484,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -1472,13 +1493,13 @@
         <v>5</v>
       </c>
       <c r="N14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O14">
         <v>500</v>
       </c>
       <c r="P14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q14">
         <v>2</v>
@@ -1490,18 +1511,18 @@
         <v>30.857299999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E15" s="3">
         <v>45797</v>
@@ -1522,7 +1543,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1531,13 +1552,13 @@
         <v>5</v>
       </c>
       <c r="N15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O15">
         <v>500</v>
       </c>
       <c r="P15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q15">
         <v>2</v>
@@ -1549,18 +1570,18 @@
         <v>30.857299999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E16" s="3">
         <v>45797</v>
@@ -1581,7 +1602,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K16" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -1590,13 +1611,13 @@
         <v>3</v>
       </c>
       <c r="N16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O16">
         <v>500</v>
       </c>
       <c r="P16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q16">
         <v>8</v>
@@ -1610,16 +1631,16 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E17" s="3">
         <v>45797</v>
@@ -1640,7 +1661,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L17">
         <v>1</v>
@@ -1649,13 +1670,13 @@
         <v>3</v>
       </c>
       <c r="N17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O17">
         <v>500</v>
       </c>
       <c r="P17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q17">
         <v>8</v>
@@ -1669,16 +1690,16 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E18" s="3">
         <v>45797</v>
@@ -1699,7 +1720,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -1708,13 +1729,13 @@
         <v>2</v>
       </c>
       <c r="N18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O18">
         <v>500</v>
       </c>
       <c r="P18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q18">
         <v>14</v>
@@ -1728,16 +1749,16 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E19" s="3">
         <v>45797</v>
@@ -1758,7 +1779,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K19" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -1767,13 +1788,13 @@
         <v>2</v>
       </c>
       <c r="N19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O19">
         <v>500</v>
       </c>
       <c r="P19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q19">
         <v>14</v>
@@ -1787,16 +1808,16 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E20" s="3">
         <v>45797</v>
@@ -1817,7 +1838,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -1826,13 +1847,13 @@
         <v>2</v>
       </c>
       <c r="N20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O20">
         <v>500</v>
       </c>
       <c r="P20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q20">
         <v>14</v>
@@ -1846,16 +1867,16 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E21" s="3">
         <v>45797</v>
@@ -1876,7 +1897,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -1885,13 +1906,13 @@
         <v>2</v>
       </c>
       <c r="N21" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O21">
         <v>500</v>
       </c>
       <c r="P21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q21">
         <v>14</v>
@@ -1905,16 +1926,16 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E22" s="3">
         <v>45797</v>
@@ -1935,7 +1956,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K22" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="L22">
         <v>1</v>
@@ -1944,13 +1965,13 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O22">
         <v>500</v>
       </c>
       <c r="P22" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q22">
         <v>14</v>
@@ -1964,16 +1985,16 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E23" s="3">
         <v>45797</v>
@@ -1994,7 +2015,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K23" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L23">
         <v>1</v>
@@ -2003,13 +2024,13 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O23">
         <v>500</v>
       </c>
       <c r="P23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q23">
         <v>14</v>
@@ -2023,16 +2044,16 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E24" s="3">
         <v>45797</v>
@@ -2053,7 +2074,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -2062,13 +2083,13 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O24">
         <v>500</v>
       </c>
       <c r="P24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q24">
         <v>14</v>
@@ -2082,16 +2103,16 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E25" s="3">
         <v>45797</v>
@@ -2112,7 +2133,7 @@
         <v>24.123000000000001</v>
       </c>
       <c r="K25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="L25">
         <v>1</v>
@@ -2121,13 +2142,13 @@
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O25">
         <v>500</v>
       </c>
       <c r="P25" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q25">
         <v>14</v>
@@ -2141,16 +2162,16 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E26" s="3">
         <v>45797</v>
@@ -2171,7 +2192,7 @@
         <v>25.279</v>
       </c>
       <c r="K26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L26">
         <v>3</v>
@@ -2180,13 +2201,13 @@
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O26">
         <v>500</v>
       </c>
       <c r="P26" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="Q26">
         <v>2</v>
@@ -2200,16 +2221,16 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E27" s="3">
         <v>45797</v>
@@ -2230,7 +2251,7 @@
         <v>25.279</v>
       </c>
       <c r="K27" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L27">
         <v>3</v>
@@ -2239,13 +2260,13 @@
         <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O27">
         <v>500</v>
       </c>
       <c r="P27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="Q27">
         <v>2</v>
@@ -2259,16 +2280,16 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E28" s="3">
         <v>45797</v>
@@ -2289,7 +2310,7 @@
         <v>25.279</v>
       </c>
       <c r="K28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="L28">
         <v>3</v>
@@ -2298,13 +2319,13 @@
         <v>3</v>
       </c>
       <c r="N28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O28">
         <v>500</v>
       </c>
       <c r="P28" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q28">
         <v>8</v>
@@ -2318,16 +2339,16 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E29" s="3">
         <v>45797</v>
@@ -2348,7 +2369,7 @@
         <v>25.279</v>
       </c>
       <c r="K29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L29">
         <v>3</v>
@@ -2357,13 +2378,13 @@
         <v>3</v>
       </c>
       <c r="N29" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O29">
         <v>500</v>
       </c>
       <c r="P29" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q29">
         <v>8</v>
@@ -2377,16 +2398,16 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E30" s="3">
         <v>45797</v>
@@ -2407,7 +2428,7 @@
         <v>25.279</v>
       </c>
       <c r="K30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L30">
         <v>3</v>
@@ -2416,13 +2437,13 @@
         <v>2</v>
       </c>
       <c r="N30" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O30">
         <v>500</v>
       </c>
       <c r="P30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q30">
         <v>14</v>
@@ -2436,16 +2457,16 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E31" s="3">
         <v>45797</v>
@@ -2466,7 +2487,7 @@
         <v>25.279</v>
       </c>
       <c r="K31" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L31">
         <v>3</v>
@@ -2475,13 +2496,13 @@
         <v>2</v>
       </c>
       <c r="N31" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O31">
         <v>500</v>
       </c>
       <c r="P31" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q31">
         <v>14</v>
@@ -2495,16 +2516,16 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E32" s="3">
         <v>45797</v>
@@ -2525,7 +2546,7 @@
         <v>25.279</v>
       </c>
       <c r="K32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L32">
         <v>3</v>
@@ -2534,13 +2555,13 @@
         <v>2</v>
       </c>
       <c r="N32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O32">
         <v>500</v>
       </c>
       <c r="P32" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q32">
         <v>14</v>
@@ -2554,16 +2575,16 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E33" s="3">
         <v>45797</v>
@@ -2584,7 +2605,7 @@
         <v>25.279</v>
       </c>
       <c r="K33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L33">
         <v>3</v>
@@ -2593,13 +2614,13 @@
         <v>2</v>
       </c>
       <c r="N33" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O33">
         <v>500</v>
       </c>
       <c r="P33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q33">
         <v>14</v>
@@ -2613,16 +2634,16 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E34" s="3">
         <v>45797</v>
@@ -2643,7 +2664,7 @@
         <v>25.279</v>
       </c>
       <c r="K34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L34">
         <v>3</v>
@@ -2652,13 +2673,13 @@
         <v>1</v>
       </c>
       <c r="N34" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O34">
         <v>500</v>
       </c>
       <c r="P34" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q34">
         <v>14</v>
@@ -2672,16 +2693,16 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E35" s="3">
         <v>45797</v>
@@ -2702,7 +2723,7 @@
         <v>25.279</v>
       </c>
       <c r="K35" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="L35">
         <v>3</v>
@@ -2711,13 +2732,13 @@
         <v>1</v>
       </c>
       <c r="N35" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O35">
         <v>500</v>
       </c>
       <c r="P35" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q35">
         <v>14</v>
@@ -2731,16 +2752,16 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E36" s="3">
         <v>45797</v>
@@ -2761,7 +2782,7 @@
         <v>25.279</v>
       </c>
       <c r="K36" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L36">
         <v>3</v>
@@ -2770,13 +2791,13 @@
         <v>1</v>
       </c>
       <c r="N36" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O36">
         <v>500</v>
       </c>
       <c r="P36" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q36">
         <v>14</v>
@@ -2790,16 +2811,16 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E37" s="3">
         <v>45797</v>
@@ -2820,7 +2841,7 @@
         <v>25.279</v>
       </c>
       <c r="K37" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="L37">
         <v>3</v>
@@ -2829,13 +2850,13 @@
         <v>1</v>
       </c>
       <c r="N37" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O37">
         <v>500</v>
       </c>
       <c r="P37" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="Q37">
         <v>14</v>

</xml_diff>

<commit_message>
no need to correct for salinity
- salinity is used in the pH calculation so no need to correct for it (when correcting for in situ temperature and pressure)
</commit_message>
<xml_diff>
--- a/pH_glider/water_sampling/sample_logs/RMI2_pH_Water_Sample_Log.xlsx
+++ b/pH_glider/water_sampling/sample_logs/RMI2_pH_Water_Sample_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garzio/Documents/repo/rucool/dataset_archiving/pH_glider/water_sampling/sample_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CB1D65-A1C4-714D-B3AA-25FD973DCAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD1856B-1501-A644-8F6F-8C5A2C21C403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="800" windowWidth="35840" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="21500" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleLog" sheetId="1" r:id="rId1"/>
@@ -533,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -559,7 +559,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,9 +841,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4047,7 +4046,7 @@
       <c r="P40" s="5">
         <v>500</v>
       </c>
-      <c r="Q40" s="20" t="s">
+      <c r="Q40" t="s">
         <v>113</v>
       </c>
       <c r="R40" s="5">
@@ -4112,7 +4111,7 @@
       <c r="P41">
         <v>500</v>
       </c>
-      <c r="Q41" s="20" t="s">
+      <c r="Q41" t="s">
         <v>113</v>
       </c>
       <c r="R41">
@@ -4252,7 +4251,7 @@
       <c r="P43" s="5">
         <v>500</v>
       </c>
-      <c r="Q43" s="20" t="s">
+      <c r="Q43" t="s">
         <v>113</v>
       </c>
       <c r="R43" s="5">
@@ -4317,7 +4316,7 @@
       <c r="P44">
         <v>500</v>
       </c>
-      <c r="Q44" s="20" t="s">
+      <c r="Q44" t="s">
         <v>113</v>
       </c>
       <c r="R44">
@@ -4457,7 +4456,7 @@
       <c r="P46" s="5">
         <v>500</v>
       </c>
-      <c r="Q46" s="20" t="s">
+      <c r="Q46" t="s">
         <v>113</v>
       </c>
       <c r="R46" s="5">
@@ -4522,7 +4521,7 @@
       <c r="P47">
         <v>500</v>
       </c>
-      <c r="Q47" s="20" t="s">
+      <c r="Q47" t="s">
         <v>113</v>
       </c>
       <c r="R47">
@@ -4662,7 +4661,7 @@
       <c r="P49" s="5">
         <v>500</v>
       </c>
-      <c r="Q49" s="20" t="s">
+      <c r="Q49" t="s">
         <v>113</v>
       </c>
       <c r="R49" s="5">
@@ -4727,7 +4726,7 @@
       <c r="P50">
         <v>500</v>
       </c>
-      <c r="Q50" s="20" t="s">
+      <c r="Q50" t="s">
         <v>113</v>
       </c>
       <c r="R50">
@@ -4867,7 +4866,6 @@
       <c r="P52" s="5">
         <v>500</v>
       </c>
-      <c r="Q52" s="20"/>
       <c r="R52" s="5">
         <v>10</v>
       </c>

</xml_diff>